<commit_message>
[UPD] Poprawiono sposób liczenia Calmar dla wyników "konkursu"
</commit_message>
<xml_diff>
--- a/Results/AS/wyniki.xlsx
+++ b/Results/AS/wyniki.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="109">
   <si>
     <t>nr testu</t>
   </si>
@@ -329,14 +329,26 @@
     <t>Obsunięcia kapitału</t>
   </si>
   <si>
-    <t>Calmar Ratio</t>
+    <t>Calmar Ratio1</t>
+  </si>
+  <si>
+    <t>Zysk skumulowany</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>Calmar Ratio2</t>
+  </si>
+  <si>
+    <t>źle liczony</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +370,13 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -373,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -636,11 +655,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -708,8 +758,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -741,6 +789,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1035,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1053,7 +1117,7 @@
     <col min="10" max="10" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1078,13 +1142,23 @@
       <c r="H1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="42" t="s">
+      <c r="J1" s="39"/>
+      <c r="K1" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="L1" s="43"/>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="L1" s="41"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" s="41"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="R1" s="41"/>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -1109,7 +1183,7 @@
       <c r="H2" s="20">
         <v>0.30449999999999999</v>
       </c>
-      <c r="J2" s="33">
+      <c r="J2" s="31">
         <f>ABS(E2-E3)</f>
         <v>0</v>
       </c>
@@ -1117,12 +1191,36 @@
         <f t="shared" ref="K2:L2" si="0">ABS(F2-F3)</f>
         <v>1.2299999999999998E-2</v>
       </c>
-      <c r="L2" s="34">
+      <c r="L2" s="1">
         <f t="shared" si="0"/>
         <v>8.4000000000000047E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="42">
+        <f>E2</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="43">
+        <f t="shared" ref="N2:O2" si="1">F2</f>
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="O2" s="44">
+        <f t="shared" si="1"/>
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="P2" s="42">
+        <f>M2-MAX(M2:M2)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="43">
+        <f t="shared" ref="Q2:R2" si="2">N2-MAX(N2:N2)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1147,20 +1245,44 @@
       <c r="H3" s="13">
         <v>0.17369999999999999</v>
       </c>
-      <c r="J3" s="33">
-        <f t="shared" ref="J3:J35" si="1">ABS(E3-E4)</f>
+      <c r="J3" s="31">
+        <f t="shared" ref="J3:J34" si="3">ABS(E3-E4)</f>
         <v>3.61E-2</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K27" si="2">ABS(F3-F4)</f>
+        <f t="shared" ref="K3:K27" si="4">ABS(F3-F4)</f>
         <v>2.9100000000000001E-2</v>
       </c>
-      <c r="L3" s="34">
-        <f t="shared" ref="L3:L27" si="3">ABS(G3-G4)</f>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L27" si="5">ABS(G3-G4)</f>
         <v>2.4300000000000002E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="31">
+        <f>M2+E3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" ref="N3:O18" si="6">N2+F3</f>
+        <v>8.1699999999999995E-2</v>
+      </c>
+      <c r="O3" s="32">
+        <f t="shared" si="6"/>
+        <v>9.64E-2</v>
+      </c>
+      <c r="P3" s="31">
+        <f>M3-MAX(M2:M3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <f t="shared" ref="Q3:R3" si="7">N3-MAX(N2:N3)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="32">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1185,20 +1307,44 @@
       <c r="H4" s="13">
         <v>8.1500000000000003E-2</v>
       </c>
-      <c r="J4" s="33">
-        <f t="shared" si="1"/>
+      <c r="J4" s="31">
+        <f t="shared" si="3"/>
         <v>5.4300000000000001E-2</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="L4" s="34">
-        <f t="shared" si="3"/>
+      <c r="L4" s="1">
+        <f t="shared" si="5"/>
         <v>1.0200000000000001E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="31">
+        <f>M3+E4</f>
+        <v>3.61E-2</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="6"/>
+        <v>9.9599999999999994E-2</v>
+      </c>
+      <c r="O4" s="32">
+        <f t="shared" si="6"/>
+        <v>0.1731</v>
+      </c>
+      <c r="P4" s="31">
+        <f>M4-MAX(M2:M4)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ref="Q4:R4" si="8">N4-MAX(N2:N4)</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="32">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1211,7 +1357,7 @@
       <c r="D5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="25">
         <v>-1.8200000000000001E-2</v>
       </c>
       <c r="F5" s="2">
@@ -1223,20 +1369,44 @@
       <c r="H5" s="13">
         <v>0.10009999999999999</v>
       </c>
-      <c r="J5" s="33">
-        <f t="shared" si="1"/>
+      <c r="J5" s="31">
+        <f t="shared" si="3"/>
         <v>2.4300000000000002E-2</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.1299999999999999E-2</v>
       </c>
-      <c r="L5" s="34">
-        <f t="shared" si="3"/>
+      <c r="L5" s="1">
+        <f t="shared" si="5"/>
         <v>1.1000000000000003E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="31">
+        <f t="shared" ref="M5:M25" si="9">M4+E5</f>
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="6"/>
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="O5" s="32">
+        <f t="shared" si="6"/>
+        <v>0.23960000000000001</v>
+      </c>
+      <c r="P5" s="31">
+        <f>M5-MAX(M2:M5)</f>
+        <v>-1.8200000000000001E-2</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" ref="Q5:R5" si="10">N5-MAX(N2:N5)</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="32">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1261,20 +1431,44 @@
       <c r="H6" s="13">
         <v>3.4500000000000003E-2</v>
       </c>
-      <c r="J6" s="33">
-        <f t="shared" si="1"/>
+      <c r="J6" s="31">
+        <f t="shared" si="3"/>
         <v>1.5299999999999998E-2</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.4499999999999999E-2</v>
       </c>
-      <c r="L6" s="34">
-        <f t="shared" si="3"/>
+      <c r="L6" s="1">
+        <f t="shared" si="5"/>
         <v>9.5000000000000015E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="31">
+        <f t="shared" si="9"/>
+        <v>2.4E-2</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="6"/>
+        <v>0.12669999999999998</v>
+      </c>
+      <c r="O6" s="32">
+        <f t="shared" si="6"/>
+        <v>0.29510000000000003</v>
+      </c>
+      <c r="P6" s="31">
+        <f>M6-MAX(M2:M6)</f>
+        <v>-1.21E-2</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" ref="Q6:R6" si="11">N6-MAX(N2:N6)</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="32">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1299,20 +1493,44 @@
       <c r="H7" s="13">
         <v>6.2300000000000001E-2</v>
       </c>
-      <c r="J7" s="33">
-        <f t="shared" si="1"/>
+      <c r="J7" s="31">
+        <f t="shared" si="3"/>
         <v>1.24E-2</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5000000000000013E-3</v>
       </c>
-      <c r="L7" s="34">
-        <f t="shared" si="3"/>
+      <c r="L7" s="1">
+        <f t="shared" si="5"/>
         <v>2.6199999999999998E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="31">
+        <f t="shared" si="9"/>
+        <v>4.5399999999999996E-2</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="6"/>
+        <v>0.16539999999999999</v>
+      </c>
+      <c r="O7" s="32">
+        <f t="shared" si="6"/>
+        <v>0.34110000000000001</v>
+      </c>
+      <c r="P7" s="31">
+        <f>M7-MAX(M2:M7)</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" ref="Q7:R7" si="12">N7-MAX(N2:N7)</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="32">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1337,20 +1555,44 @@
       <c r="H8" s="13">
         <v>6.4699999999999994E-2</v>
       </c>
-      <c r="J8" s="33">
-        <f t="shared" si="1"/>
+      <c r="J8" s="31">
+        <f t="shared" si="3"/>
         <v>6.6999999999999994E-3</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5799999999999997E-2</v>
       </c>
-      <c r="L8" s="34">
-        <f t="shared" si="3"/>
+      <c r="L8" s="1">
+        <f t="shared" si="5"/>
         <v>7.5300000000000006E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="31">
+        <f t="shared" si="9"/>
+        <v>5.4399999999999997E-2</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="6"/>
+        <v>0.2026</v>
+      </c>
+      <c r="O8" s="32">
+        <f t="shared" si="6"/>
+        <v>0.3609</v>
+      </c>
+      <c r="P8" s="31">
+        <f>M8-MAX(M2:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" ref="Q8:R8" si="13">N8-MAX(N2:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="32">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1369,26 +1611,50 @@
       <c r="F9" s="2">
         <v>1.14E-2</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="26">
         <v>-5.5500000000000001E-2</v>
       </c>
       <c r="H9" s="13">
         <v>7.3099999999999998E-2</v>
       </c>
-      <c r="J9" s="33">
-        <f t="shared" si="1"/>
+      <c r="J9" s="31">
+        <f t="shared" si="3"/>
         <v>8.000000000000021E-4</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.2299999999999995E-2</v>
       </c>
-      <c r="L9" s="34">
-        <f t="shared" si="3"/>
+      <c r="L9" s="1">
+        <f t="shared" si="5"/>
         <v>6.359999999999999E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" s="31">
+        <f t="shared" si="9"/>
+        <v>7.0099999999999996E-2</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="6"/>
+        <v>0.214</v>
+      </c>
+      <c r="O9" s="32">
+        <f t="shared" si="6"/>
+        <v>0.3054</v>
+      </c>
+      <c r="P9" s="31">
+        <f>M9-MAX(M2:M9)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" ref="Q9:R9" si="14">N9-MAX(N2:N9)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="32">
+        <f t="shared" si="14"/>
+        <v>-5.5499999999999994E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1404,29 +1670,53 @@
       <c r="E10" s="7">
         <v>1.6500000000000001E-2</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="27">
         <v>-2.0899999999999998E-2</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="26">
         <v>-0.1191</v>
       </c>
       <c r="H10" s="13">
         <v>0.11890000000000001</v>
       </c>
-      <c r="J10" s="33">
-        <f t="shared" si="1"/>
+      <c r="J10" s="31">
+        <f t="shared" si="3"/>
         <v>1.9700000000000002E-2</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.3099999999999999E-2</v>
       </c>
-      <c r="L10" s="34">
-        <f t="shared" si="3"/>
+      <c r="L10" s="1">
+        <f t="shared" si="5"/>
         <v>0.1027</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="31">
+        <f t="shared" si="9"/>
+        <v>8.6599999999999996E-2</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="6"/>
+        <v>0.19309999999999999</v>
+      </c>
+      <c r="O10" s="32">
+        <f t="shared" si="6"/>
+        <v>0.18630000000000002</v>
+      </c>
+      <c r="P10" s="31">
+        <f>M10-MAX(M2:M10)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" ref="Q10:R10" si="15">N10-MAX(N2:N10)</f>
+        <v>-2.0900000000000002E-2</v>
+      </c>
+      <c r="R10" s="32">
+        <f t="shared" si="15"/>
+        <v>-0.17459999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1439,32 +1729,56 @@
       <c r="D11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="25">
         <v>-3.2000000000000002E-3</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="27">
         <v>-7.7999999999999996E-3</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="26">
         <v>-1.6400000000000001E-2</v>
       </c>
       <c r="H11" s="13">
         <v>0.13619999999999999</v>
       </c>
-      <c r="J11" s="33">
-        <f t="shared" si="1"/>
+      <c r="J11" s="31">
+        <f t="shared" si="3"/>
         <v>4.0800000000000003E-2</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.5600000000000001E-2</v>
       </c>
-      <c r="L11" s="34">
-        <f t="shared" si="3"/>
+      <c r="L11" s="1">
+        <f t="shared" si="5"/>
         <v>3.4100000000000005E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" s="31">
+        <f t="shared" si="9"/>
+        <v>8.3400000000000002E-2</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="6"/>
+        <v>0.18529999999999999</v>
+      </c>
+      <c r="O11" s="32">
+        <f t="shared" si="6"/>
+        <v>0.16990000000000002</v>
+      </c>
+      <c r="P11" s="31">
+        <f>M11-MAX(M$2:M11)</f>
+        <v>-3.1999999999999945E-3</v>
+      </c>
+      <c r="Q11" s="1">
+        <f>N11-MAX(N$2:N11)</f>
+        <v>-2.8700000000000003E-2</v>
+      </c>
+      <c r="R11" s="32">
+        <f>O11-MAX(O$2:O11)</f>
+        <v>-0.19099999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1480,7 +1794,7 @@
       <c r="E12" s="7">
         <v>3.7600000000000001E-2</v>
       </c>
-      <c r="F12" s="29">
+      <c r="F12" s="27">
         <v>-8.3400000000000002E-2</v>
       </c>
       <c r="G12" s="3">
@@ -1489,20 +1803,44 @@
       <c r="H12" s="13">
         <v>0.1953</v>
       </c>
-      <c r="J12" s="33">
-        <f t="shared" si="1"/>
+      <c r="J12" s="31">
+        <f t="shared" si="3"/>
         <v>0.11149999999999999</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.3E-3</v>
       </c>
-      <c r="L12" s="34">
-        <f t="shared" si="3"/>
+      <c r="L12" s="1">
+        <f t="shared" si="5"/>
         <v>2.1100000000000001E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" s="31">
+        <f t="shared" si="9"/>
+        <v>0.121</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="6"/>
+        <v>0.10189999999999999</v>
+      </c>
+      <c r="O12" s="32">
+        <f t="shared" si="6"/>
+        <v>0.18760000000000002</v>
+      </c>
+      <c r="P12" s="31">
+        <f>M12-MAX(M$2:M12)</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <f>N12-MAX(N$2:N12)</f>
+        <v>-0.11210000000000001</v>
+      </c>
+      <c r="R12" s="32">
+        <f>O12-MAX(O$2:O12)</f>
+        <v>-0.17329999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1515,45 +1853,69 @@
       <c r="D13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="25">
         <v>-7.3899999999999993E-2</v>
       </c>
-      <c r="F13" s="29">
+      <c r="F13" s="27">
         <v>-7.7100000000000002E-2</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="26">
         <v>-3.3999999999999998E-3</v>
       </c>
       <c r="H13" s="13">
         <v>8.7599999999999997E-2</v>
       </c>
-      <c r="J13" s="33">
-        <f t="shared" si="1"/>
+      <c r="J13" s="31">
+        <f t="shared" si="3"/>
         <v>3.3199999999999993E-2</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.1013</v>
       </c>
-      <c r="L13" s="34">
-        <f t="shared" si="3"/>
+      <c r="L13" s="1">
+        <f t="shared" si="5"/>
         <v>0.11890000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" s="31">
+        <f t="shared" si="9"/>
+        <v>4.7100000000000003E-2</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="6"/>
+        <v>2.4799999999999989E-2</v>
+      </c>
+      <c r="O13" s="32">
+        <f t="shared" si="6"/>
+        <v>0.18420000000000003</v>
+      </c>
+      <c r="P13" s="31">
+        <f>M13-MAX(M$2:M13)</f>
+        <v>-7.3899999999999993E-2</v>
+      </c>
+      <c r="Q13" s="1">
+        <f>N13-MAX(N$2:N13)</f>
+        <v>-0.18920000000000001</v>
+      </c>
+      <c r="R13" s="32">
+        <f>O13-MAX(O$2:O13)</f>
+        <v>-0.17669999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="27">
         <v>-4.3E-3</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="25">
         <v>-4.07E-2</v>
       </c>
       <c r="F14" s="2">
@@ -1562,23 +1924,47 @@
       <c r="G14" s="3">
         <v>0.11550000000000001</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="28">
         <v>-5.5999999999999995E-4</v>
       </c>
-      <c r="J14" s="33">
-        <f t="shared" si="1"/>
+      <c r="J14" s="31">
+        <f t="shared" si="3"/>
         <v>7.980000000000001E-2</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.8400000000000004E-2</v>
       </c>
-      <c r="L14" s="34">
-        <f t="shared" si="3"/>
+      <c r="L14" s="1">
+        <f t="shared" si="5"/>
         <v>2.7200000000000002E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" s="31">
+        <f t="shared" si="9"/>
+        <v>6.4000000000000029E-3</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="6"/>
+        <v>4.8999999999999988E-2</v>
+      </c>
+      <c r="O14" s="32">
+        <f t="shared" si="6"/>
+        <v>0.29970000000000002</v>
+      </c>
+      <c r="P14" s="31">
+        <f>M14-MAX(M$2:M14)</f>
+        <v>-0.11459999999999999</v>
+      </c>
+      <c r="Q14" s="1">
+        <f>N14-MAX(N$2:N14)</f>
+        <v>-0.16500000000000001</v>
+      </c>
+      <c r="R14" s="32">
+        <f>O14-MAX(O$2:O14)</f>
+        <v>-6.1199999999999977E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1603,20 +1989,44 @@
       <c r="H15" s="13">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="J15" s="33">
-        <f t="shared" si="1"/>
+      <c r="J15" s="31">
+        <f t="shared" si="3"/>
         <v>3.0000000000000165E-4</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.3800000000000002E-2</v>
       </c>
-      <c r="L15" s="34">
-        <f t="shared" si="3"/>
+      <c r="L15" s="1">
+        <f t="shared" si="5"/>
         <v>0.10540000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" s="31">
+        <f t="shared" si="9"/>
+        <v>4.5500000000000006E-2</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="6"/>
+        <v>0.11159999999999999</v>
+      </c>
+      <c r="O15" s="32">
+        <f t="shared" si="6"/>
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="P15" s="31">
+        <f>M15-MAX(M$2:M15)</f>
+        <v>-7.5499999999999984E-2</v>
+      </c>
+      <c r="Q15" s="1">
+        <f>N15-MAX(N$2:N15)</f>
+        <v>-0.1024</v>
+      </c>
+      <c r="R15" s="32">
+        <f>O15-MAX(O$2:O15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -1635,26 +2045,50 @@
       <c r="F16" s="2">
         <v>3.8800000000000001E-2</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="26">
         <v>-1.7100000000000001E-2</v>
       </c>
       <c r="H16" s="13">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="J16" s="33">
-        <f t="shared" si="1"/>
+      <c r="J16" s="31">
+        <f t="shared" si="3"/>
         <v>3.8800000000000001E-2</v>
       </c>
       <c r="K16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.8600000000000002E-2</v>
       </c>
-      <c r="L16" s="34">
-        <f t="shared" si="3"/>
+      <c r="L16" s="1">
+        <f t="shared" si="5"/>
         <v>5.1900000000000002E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="31">
+        <f t="shared" si="9"/>
+        <v>8.4300000000000014E-2</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="6"/>
+        <v>0.15039999999999998</v>
+      </c>
+      <c r="O16" s="32">
+        <f t="shared" si="6"/>
+        <v>0.37090000000000001</v>
+      </c>
+      <c r="P16" s="31">
+        <f>M16-MAX(M$2:M16)</f>
+        <v>-3.6699999999999983E-2</v>
+      </c>
+      <c r="Q16" s="1">
+        <f>N16-MAX(N$2:N16)</f>
+        <v>-6.3600000000000018E-2</v>
+      </c>
+      <c r="R16" s="32">
+        <f>O16-MAX(O$2:O16)</f>
+        <v>-1.7100000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -1673,26 +2107,50 @@
       <c r="F17" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G17" s="28">
+      <c r="G17" s="26">
         <v>-6.9000000000000006E-2</v>
       </c>
       <c r="H17" s="13">
         <v>8.9700000000000002E-2</v>
       </c>
-      <c r="J17" s="33">
-        <f t="shared" si="1"/>
+      <c r="J17" s="31">
+        <f t="shared" si="3"/>
         <v>3.2000000000000003E-4</v>
       </c>
       <c r="K17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.0000000000000006E-4</v>
       </c>
-      <c r="L17" s="34">
-        <f t="shared" si="3"/>
+      <c r="L17" s="1">
+        <f t="shared" si="5"/>
         <v>9.900000000000006E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="31">
+        <f t="shared" si="9"/>
+        <v>8.4300000000000014E-2</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="6"/>
+        <v>0.15059999999999998</v>
+      </c>
+      <c r="O17" s="32">
+        <f t="shared" si="6"/>
+        <v>0.3019</v>
+      </c>
+      <c r="P17" s="31">
+        <f>M17-MAX(M$2:M17)</f>
+        <v>-3.6699999999999983E-2</v>
+      </c>
+      <c r="Q17" s="1">
+        <f>N17-MAX(N$2:N17)</f>
+        <v>-6.3400000000000012E-2</v>
+      </c>
+      <c r="R17" s="32">
+        <f>O17-MAX(O$2:O17)</f>
+        <v>-8.610000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -1711,26 +2169,50 @@
       <c r="F18" s="2">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="26">
         <v>-5.91E-2</v>
       </c>
       <c r="H18" s="13">
         <v>8.0100000000000005E-2</v>
       </c>
-      <c r="J18" s="33">
-        <f t="shared" si="1"/>
+      <c r="J18" s="31">
+        <f t="shared" si="3"/>
         <v>8.5799999999999991E-3</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.8500000000000001E-2</v>
       </c>
-      <c r="L18" s="34">
-        <f t="shared" si="3"/>
+      <c r="L18" s="1">
+        <f t="shared" si="5"/>
         <v>3.0000000000000165E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="31">
+        <f t="shared" si="9"/>
+        <v>8.4620000000000015E-2</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="6"/>
+        <v>0.15139999999999998</v>
+      </c>
+      <c r="O18" s="32">
+        <f t="shared" si="6"/>
+        <v>0.24280000000000002</v>
+      </c>
+      <c r="P18" s="31">
+        <f>M18-MAX(M$2:M18)</f>
+        <v>-3.6379999999999982E-2</v>
+      </c>
+      <c r="Q18" s="1">
+        <f>N18-MAX(N$2:N18)</f>
+        <v>-6.2600000000000017E-2</v>
+      </c>
+      <c r="R18" s="32">
+        <f>O18-MAX(O$2:O18)</f>
+        <v>-0.1452</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -1746,29 +2228,53 @@
       <c r="E19" s="7">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="F19" s="29">
+      <c r="F19" s="27">
         <v>-4.7699999999999999E-2</v>
       </c>
-      <c r="G19" s="28">
+      <c r="G19" s="26">
         <v>-5.8799999999999998E-2</v>
       </c>
       <c r="H19" s="13">
         <v>6.0400000000000002E-2</v>
       </c>
-      <c r="J19" s="33">
-        <f t="shared" si="1"/>
+      <c r="J19" s="31">
+        <f t="shared" si="3"/>
         <v>7.9700000000000007E-2</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.4200000000000005E-2</v>
       </c>
-      <c r="L19" s="34">
-        <f t="shared" si="3"/>
+      <c r="L19" s="1">
+        <f t="shared" si="5"/>
         <v>8.1200000000000022E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="31">
+        <f t="shared" si="9"/>
+        <v>9.352000000000002E-2</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" ref="N19:N35" si="16">N18+F19</f>
+        <v>0.10369999999999999</v>
+      </c>
+      <c r="O19" s="32">
+        <f t="shared" ref="O19:O35" si="17">O18+G19</f>
+        <v>0.18400000000000002</v>
+      </c>
+      <c r="P19" s="31">
+        <f>M19-MAX(M$2:M19)</f>
+        <v>-2.7479999999999977E-2</v>
+      </c>
+      <c r="Q19" s="1">
+        <f>N19-MAX(N$2:N19)</f>
+        <v>-0.11030000000000001</v>
+      </c>
+      <c r="R19" s="32">
+        <f>O19-MAX(O$2:O19)</f>
+        <v>-0.20399999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -1781,32 +2287,56 @@
       <c r="D20" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="25">
         <v>-7.0800000000000002E-2</v>
       </c>
-      <c r="F20" s="29">
+      <c r="F20" s="27">
         <v>-0.1019</v>
       </c>
-      <c r="G20" s="28">
+      <c r="G20" s="26">
         <v>-0.14000000000000001</v>
       </c>
       <c r="H20" s="13">
         <v>8.9800000000000005E-2</v>
       </c>
-      <c r="J20" s="33">
-        <f t="shared" si="1"/>
+      <c r="J20" s="31">
+        <f t="shared" si="3"/>
         <v>4.7899999999999998E-2</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.7800000000000003E-2</v>
       </c>
-      <c r="L20" s="34">
-        <f t="shared" si="3"/>
+      <c r="L20" s="1">
+        <f t="shared" si="5"/>
         <v>0.10100000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" s="31">
+        <f t="shared" si="9"/>
+        <v>2.2720000000000018E-2</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="16"/>
+        <v>1.7999999999999822E-3</v>
+      </c>
+      <c r="O20" s="32">
+        <f t="shared" si="17"/>
+        <v>4.4000000000000011E-2</v>
+      </c>
+      <c r="P20" s="31">
+        <f>M20-MAX(M$2:M20)</f>
+        <v>-9.8279999999999978E-2</v>
+      </c>
+      <c r="Q20" s="1">
+        <f>N20-MAX(N$2:N20)</f>
+        <v>-0.2122</v>
+      </c>
+      <c r="R20" s="32">
+        <f>O20-MAX(O$2:O20)</f>
+        <v>-0.34399999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -1819,32 +2349,56 @@
       <c r="D21" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="25">
         <v>-2.29E-2</v>
       </c>
-      <c r="F21" s="29">
+      <c r="F21" s="27">
         <v>-1.41E-2</v>
       </c>
-      <c r="G21" s="28">
+      <c r="G21" s="26">
         <v>-3.9E-2</v>
       </c>
       <c r="H21" s="13">
         <v>4.02E-2</v>
       </c>
-      <c r="J21" s="33">
-        <f t="shared" si="1"/>
+      <c r="J21" s="31">
+        <f t="shared" si="3"/>
         <v>5.7700000000000001E-2</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="L21" s="34">
-        <f t="shared" si="3"/>
+      <c r="L21" s="1">
+        <f t="shared" si="5"/>
         <v>0.11579999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="31">
+        <f t="shared" si="9"/>
+        <v>-1.7999999999998226E-4</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="16"/>
+        <v>-1.2300000000000018E-2</v>
+      </c>
+      <c r="O21" s="32">
+        <f t="shared" si="17"/>
+        <v>5.0000000000000114E-3</v>
+      </c>
+      <c r="P21" s="31">
+        <f>M21-MAX(M$2:M21)</f>
+        <v>-0.12117999999999998</v>
+      </c>
+      <c r="Q21" s="1">
+        <f>N21-MAX(N$2:N21)</f>
+        <v>-0.2263</v>
+      </c>
+      <c r="R21" s="32">
+        <f>O21-MAX(O$2:O21)</f>
+        <v>-0.38300000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -1869,20 +2423,44 @@
       <c r="H22" s="13">
         <v>9.0800000000000006E-2</v>
       </c>
-      <c r="J22" s="33">
-        <f t="shared" si="1"/>
+      <c r="J22" s="31">
+        <f t="shared" si="3"/>
         <v>4.8599999999999997E-2</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.3700000000000002E-2</v>
       </c>
-      <c r="L22" s="34">
-        <f t="shared" si="3"/>
+      <c r="L22" s="1">
+        <f t="shared" si="5"/>
         <v>5.0199999999999995E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="31">
+        <f t="shared" si="9"/>
+        <v>3.4620000000000012E-2</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="16"/>
+        <v>8.6999999999999838E-3</v>
+      </c>
+      <c r="O22" s="32">
+        <f t="shared" si="17"/>
+        <v>8.1800000000000012E-2</v>
+      </c>
+      <c r="P22" s="31">
+        <f>M22-MAX(M$2:M22)</f>
+        <v>-8.6379999999999985E-2</v>
+      </c>
+      <c r="Q22" s="1">
+        <f>N22-MAX(N$2:N22)</f>
+        <v>-0.20530000000000001</v>
+      </c>
+      <c r="R22" s="32">
+        <f>O22-MAX(O$2:O22)</f>
+        <v>-0.30620000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -1895,10 +2473,10 @@
       <c r="D23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="25">
         <v>-1.38E-2</v>
       </c>
-      <c r="F23" s="29">
+      <c r="F23" s="27">
         <v>-2.7000000000000001E-3</v>
       </c>
       <c r="G23" s="3">
@@ -1907,20 +2485,44 @@
       <c r="H23" s="13">
         <v>8.6099999999999996E-2</v>
       </c>
-      <c r="J23" s="33">
-        <f t="shared" si="1"/>
+      <c r="J23" s="31">
+        <f t="shared" si="3"/>
         <v>3.6699999999999997E-2</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.3899999999999993E-2</v>
       </c>
-      <c r="L23" s="34">
-        <f t="shared" si="3"/>
+      <c r="L23" s="1">
+        <f t="shared" si="5"/>
         <v>3.5400000000000001E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" s="31">
+        <f t="shared" si="9"/>
+        <v>2.0820000000000012E-2</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="16"/>
+        <v>5.9999999999999836E-3</v>
+      </c>
+      <c r="O23" s="32">
+        <f t="shared" si="17"/>
+        <v>0.10840000000000001</v>
+      </c>
+      <c r="P23" s="31">
+        <f>M23-MAX(M$2:M23)</f>
+        <v>-0.10017999999999999</v>
+      </c>
+      <c r="Q23" s="1">
+        <f>N23-MAX(N$2:N23)</f>
+        <v>-0.20800000000000002</v>
+      </c>
+      <c r="R23" s="32">
+        <f>O23-MAX(O$2:O23)</f>
+        <v>-0.27960000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -1945,20 +2547,44 @@
       <c r="H24" s="13">
         <v>0.1502</v>
       </c>
-      <c r="J24" s="33">
-        <f t="shared" si="1"/>
+      <c r="J24" s="31">
+        <f t="shared" si="3"/>
         <v>2.1000000000000012E-3</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.0699999999999997E-2</v>
       </c>
-      <c r="L24" s="34">
-        <f t="shared" si="3"/>
+      <c r="L24" s="1">
+        <f t="shared" si="5"/>
         <v>5.2400000000000002E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" s="31">
+        <f t="shared" si="9"/>
+        <v>4.3720000000000009E-2</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="16"/>
+        <v>7.7199999999999977E-2</v>
+      </c>
+      <c r="O24" s="32">
+        <f t="shared" si="17"/>
+        <v>0.1704</v>
+      </c>
+      <c r="P24" s="31">
+        <f>M24-MAX(M$2:M24)</f>
+        <v>-7.7279999999999988E-2</v>
+      </c>
+      <c r="Q24" s="1">
+        <f>N24-MAX(N$2:N24)</f>
+        <v>-0.13680000000000003</v>
+      </c>
+      <c r="R24" s="32">
+        <f>O24-MAX(O$2:O24)</f>
+        <v>-0.21760000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -1983,20 +2609,44 @@
       <c r="H25" s="13">
         <v>7.17E-2</v>
       </c>
-      <c r="J25" s="33">
-        <f t="shared" si="1"/>
+      <c r="J25" s="31">
+        <f t="shared" si="3"/>
         <v>3.1099999999999999E-2</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.1600000000000001E-2</v>
       </c>
-      <c r="L25" s="34">
-        <f t="shared" si="3"/>
+      <c r="L25" s="1">
+        <f t="shared" si="5"/>
         <v>1.8799999999999997E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="31">
+        <f t="shared" si="9"/>
+        <v>6.4520000000000008E-2</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="16"/>
+        <v>8.7699999999999972E-2</v>
+      </c>
+      <c r="O25" s="32">
+        <f t="shared" si="17"/>
+        <v>0.18</v>
+      </c>
+      <c r="P25" s="31">
+        <f>M25-MAX(M$2:M25)</f>
+        <v>-5.6479999999999989E-2</v>
+      </c>
+      <c r="Q25" s="1">
+        <f>N25-MAX(N$2:N25)</f>
+        <v>-0.12630000000000002</v>
+      </c>
+      <c r="R25" s="32">
+        <f>O25-MAX(O$2:O25)</f>
+        <v>-0.20800000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -2009,32 +2659,56 @@
       <c r="D26" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E26" s="25">
         <v>-1.03E-2</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="27">
         <v>-1.1000000000000001E-3</v>
       </c>
-      <c r="G26" s="28">
+      <c r="G26" s="26">
         <v>-9.1999999999999998E-3</v>
       </c>
       <c r="H26" s="13">
         <v>5.0099999999999999E-2</v>
       </c>
-      <c r="J26" s="33">
-        <f t="shared" si="1"/>
+      <c r="J26" s="31">
+        <f t="shared" si="3"/>
         <v>2.1600000000000001E-2</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.3900000000000001E-2</v>
       </c>
-      <c r="L26" s="34">
-        <f t="shared" si="3"/>
+      <c r="L26" s="1">
+        <f t="shared" si="5"/>
         <v>4.24E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26" s="31">
+        <f>M25+E26</f>
+        <v>5.4220000000000004E-2</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" si="16"/>
+        <v>8.6599999999999969E-2</v>
+      </c>
+      <c r="O26" s="32">
+        <f t="shared" si="17"/>
+        <v>0.17080000000000001</v>
+      </c>
+      <c r="P26" s="31">
+        <f>M26-MAX(M$2:M26)</f>
+        <v>-6.6779999999999992E-2</v>
+      </c>
+      <c r="Q26" s="1">
+        <f>N26-MAX(N$2:N26)</f>
+        <v>-0.12740000000000001</v>
+      </c>
+      <c r="R26" s="32">
+        <f>O26-MAX(O$2:O26)</f>
+        <v>-0.2172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -2059,27 +2733,51 @@
       <c r="H27" s="13">
         <v>5.8500000000000003E-2</v>
       </c>
-      <c r="J27" s="33">
+      <c r="J27" s="31">
         <f>ABS(E27-E28)</f>
         <v>1.6E-2</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="L27" s="34">
-        <f t="shared" si="3"/>
+      <c r="L27" s="1">
+        <f t="shared" si="5"/>
         <v>1.5699999999999999E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" s="31">
+        <f>M26+E27</f>
+        <v>6.5520000000000009E-2</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="16"/>
+        <v>9.9399999999999974E-2</v>
+      </c>
+      <c r="O27" s="32">
+        <f t="shared" si="17"/>
+        <v>0.20400000000000001</v>
+      </c>
+      <c r="P27" s="31">
+        <f>M27-MAX(M$2:M27)</f>
+        <v>-5.5479999999999988E-2</v>
+      </c>
+      <c r="Q27" s="1">
+        <f>N27-MAX(N$2:N27)</f>
+        <v>-0.11460000000000002</v>
+      </c>
+      <c r="R27" s="32">
+        <f>O27-MAX(O$2:O27)</f>
+        <v>-0.184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="7">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="29">
+      <c r="C28" s="27">
         <v>-0.13289999999999999</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -2094,23 +2792,47 @@
       <c r="G28" s="3">
         <v>4.8899999999999999E-2</v>
       </c>
-      <c r="H28" s="30">
+      <c r="H28" s="28">
         <v>-1.04E-2</v>
       </c>
-      <c r="J28" s="33">
-        <f t="shared" si="1"/>
+      <c r="J28" s="31">
+        <f t="shared" si="3"/>
         <v>1.6100000000000003E-2</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" ref="K28:K34" si="4">ABS(F28-F29)</f>
+        <f t="shared" ref="K28:K34" si="18">ABS(F28-F29)</f>
         <v>3.1000000000000021E-3</v>
       </c>
-      <c r="L28" s="34">
-        <f t="shared" ref="L28:L34" si="5">ABS(G28-G29)</f>
+      <c r="L28" s="1">
+        <f t="shared" ref="L28:L34" si="19">ABS(G28-G29)</f>
         <v>8.3000000000000018E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" s="31">
+        <f t="shared" ref="M28:M34" si="20">M27+E28</f>
+        <v>9.2820000000000014E-2</v>
+      </c>
+      <c r="N28" s="1">
+        <f t="shared" si="16"/>
+        <v>0.12159999999999997</v>
+      </c>
+      <c r="O28" s="32">
+        <f t="shared" si="17"/>
+        <v>0.25290000000000001</v>
+      </c>
+      <c r="P28" s="31">
+        <f>M28-MAX(M$2:M28)</f>
+        <v>-2.8179999999999983E-2</v>
+      </c>
+      <c r="Q28" s="1">
+        <f>N28-MAX(N$2:N28)</f>
+        <v>-9.2400000000000024E-2</v>
+      </c>
+      <c r="R28" s="32">
+        <f>O28-MAX(O$2:O28)</f>
+        <v>-0.1351</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -2135,20 +2857,44 @@
       <c r="H29" s="13">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="J29" s="33">
-        <f t="shared" si="1"/>
+      <c r="J29" s="31">
+        <f t="shared" si="3"/>
         <v>3.7000000000000002E-3</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="18"/>
         <v>1.38E-2</v>
       </c>
-      <c r="L29" s="34">
-        <f t="shared" si="5"/>
+      <c r="L29" s="1">
+        <f t="shared" si="19"/>
         <v>2.0000000000000573E-4</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" s="31">
+        <f t="shared" si="20"/>
+        <v>0.10402000000000002</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" si="16"/>
+        <v>0.14069999999999996</v>
+      </c>
+      <c r="O29" s="32">
+        <f t="shared" si="17"/>
+        <v>0.29349999999999998</v>
+      </c>
+      <c r="P29" s="31">
+        <f>M29-MAX(M$2:M29)</f>
+        <v>-1.6979999999999981E-2</v>
+      </c>
+      <c r="Q29" s="1">
+        <f>N29-MAX(N$2:N29)</f>
+        <v>-7.3300000000000032E-2</v>
+      </c>
+      <c r="R29" s="32">
+        <f>O29-MAX(O$2:O29)</f>
+        <v>-9.4500000000000028E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -2173,20 +2919,44 @@
       <c r="H30" s="13">
         <v>1.7399999999999999E-2</v>
       </c>
-      <c r="J30" s="33">
-        <f t="shared" si="1"/>
+      <c r="J30" s="31">
+        <f t="shared" si="3"/>
         <v>9.7000000000000003E-3</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="18"/>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="L30" s="34">
-        <f t="shared" si="5"/>
+      <c r="L30" s="1">
+        <f t="shared" si="19"/>
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30" s="31">
+        <f t="shared" si="20"/>
+        <v>0.11152000000000001</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="16"/>
+        <v>0.14599999999999996</v>
+      </c>
+      <c r="O30" s="32">
+        <f t="shared" si="17"/>
+        <v>0.33429999999999999</v>
+      </c>
+      <c r="P30" s="31">
+        <f>M30-MAX(M$2:M30)</f>
+        <v>-9.4799999999999884E-3</v>
+      </c>
+      <c r="Q30" s="1">
+        <f>N30-MAX(N$2:N30)</f>
+        <v>-6.8000000000000033E-2</v>
+      </c>
+      <c r="R30" s="32">
+        <f>O30-MAX(O$2:O30)</f>
+        <v>-5.3700000000000025E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -2211,20 +2981,44 @@
       <c r="H31" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="J31" s="33">
-        <f t="shared" si="1"/>
+      <c r="J31" s="31">
+        <f t="shared" si="3"/>
         <v>1.2200000000000001E-2</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="18"/>
         <v>2.1999999999999988E-3</v>
       </c>
-      <c r="L31" s="34">
-        <f t="shared" si="5"/>
+      <c r="L31" s="1">
+        <f t="shared" si="19"/>
         <v>2.5500000000000002E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31" s="31">
+        <f t="shared" si="20"/>
+        <v>0.10932000000000001</v>
+      </c>
+      <c r="N31" s="1">
+        <f t="shared" si="16"/>
+        <v>0.15729999999999997</v>
+      </c>
+      <c r="O31" s="32">
+        <f t="shared" si="17"/>
+        <v>0.36709999999999998</v>
+      </c>
+      <c r="P31" s="31">
+        <f>M31-MAX(M$2:M31)</f>
+        <v>-1.1679999999999982E-2</v>
+      </c>
+      <c r="Q31" s="1">
+        <f>N31-MAX(N$2:N31)</f>
+        <v>-5.6700000000000028E-2</v>
+      </c>
+      <c r="R31" s="32">
+        <f>O31-MAX(O$2:O31)</f>
+        <v>-2.090000000000003E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -2249,20 +3043,44 @@
       <c r="H32" s="13">
         <v>7.3200000000000001E-2</v>
       </c>
-      <c r="J32" s="33">
-        <f t="shared" si="1"/>
+      <c r="J32" s="31">
+        <f t="shared" si="3"/>
         <v>6.2999999999999983E-3</v>
       </c>
       <c r="K32" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="18"/>
         <v>6.8999999999999999E-3</v>
       </c>
-      <c r="L32" s="34">
-        <f t="shared" si="5"/>
+      <c r="L32" s="1">
+        <f t="shared" si="19"/>
         <v>5.0700000000000002E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32" s="31">
+        <f t="shared" si="20"/>
+        <v>0.11932000000000001</v>
+      </c>
+      <c r="N32" s="1">
+        <f t="shared" si="16"/>
+        <v>0.16639999999999996</v>
+      </c>
+      <c r="O32" s="32">
+        <f t="shared" si="17"/>
+        <v>0.37439999999999996</v>
+      </c>
+      <c r="P32" s="31">
+        <f>M32-MAX(M$2:M32)</f>
+        <v>-1.6799999999999871E-3</v>
+      </c>
+      <c r="Q32" s="1">
+        <f>N32-MAX(N$2:N32)</f>
+        <v>-4.7600000000000031E-2</v>
+      </c>
+      <c r="R32" s="32">
+        <f>O32-MAX(O$2:O32)</f>
+        <v>-1.3600000000000056E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -2287,20 +3105,44 @@
       <c r="H33" s="13">
         <v>4.1799999999999997E-2</v>
       </c>
-      <c r="J33" s="33">
-        <f t="shared" si="1"/>
+      <c r="J33" s="31">
+        <f t="shared" si="3"/>
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="18"/>
         <v>2.0700000000000003E-2</v>
       </c>
-      <c r="L33" s="34">
-        <f t="shared" si="5"/>
+      <c r="L33" s="1">
+        <f t="shared" si="19"/>
         <v>1.3999999999999985E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33" s="31">
+        <f t="shared" si="20"/>
+        <v>0.13562000000000002</v>
+      </c>
+      <c r="N33" s="1">
+        <f t="shared" si="16"/>
+        <v>0.18239999999999995</v>
+      </c>
+      <c r="O33" s="32">
+        <f t="shared" si="17"/>
+        <v>0.43239999999999995</v>
+      </c>
+      <c r="P33" s="31">
+        <f>M33-MAX(M$2:M33)</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
+        <f>N33-MAX(N$2:N33)</f>
+        <v>-3.1600000000000045E-2</v>
+      </c>
+      <c r="R33" s="32">
+        <f>O33-MAX(O$2:O33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -2325,20 +3167,44 @@
       <c r="H34" s="13">
         <v>0.10780000000000001</v>
       </c>
-      <c r="J34" s="35">
-        <f t="shared" si="1"/>
+      <c r="J34" s="33">
+        <f t="shared" si="3"/>
         <v>1.2200000000000003E-2</v>
       </c>
-      <c r="K34" s="36">
-        <f t="shared" si="4"/>
+      <c r="K34" s="34">
+        <f t="shared" si="18"/>
         <v>2.1999999999999936E-3</v>
       </c>
-      <c r="L34" s="37">
-        <f t="shared" si="5"/>
+      <c r="L34" s="34">
+        <f t="shared" si="19"/>
         <v>5.9400000000000001E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="15" thickBot="1">
+      <c r="M34" s="31">
+        <f t="shared" si="20"/>
+        <v>0.15242000000000003</v>
+      </c>
+      <c r="N34" s="1">
+        <f t="shared" si="16"/>
+        <v>0.21909999999999996</v>
+      </c>
+      <c r="O34" s="32">
+        <f t="shared" si="17"/>
+        <v>0.49179999999999996</v>
+      </c>
+      <c r="P34" s="31">
+        <f>M34-MAX(M$2:M34)</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="1">
+        <f>N34-MAX(N$2:N34)</f>
+        <v>0</v>
+      </c>
+      <c r="R34" s="32">
+        <f>O34-MAX(O$2:O34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="15" thickBot="1">
       <c r="A35" s="8">
         <v>34</v>
       </c>
@@ -2357,12 +3223,36 @@
       <c r="F35" s="2">
         <v>3.8899999999999997E-2</v>
       </c>
-      <c r="G35" s="32"/>
+      <c r="G35" s="30"/>
       <c r="H35" s="14">
         <v>0.1027</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="15.75" thickBot="1">
+      <c r="M35" s="33">
+        <f>M34+E35</f>
+        <v>0.18142000000000003</v>
+      </c>
+      <c r="N35" s="34">
+        <f t="shared" si="16"/>
+        <v>0.25799999999999995</v>
+      </c>
+      <c r="O35" s="35">
+        <f t="shared" si="17"/>
+        <v>0.49179999999999996</v>
+      </c>
+      <c r="P35" s="31">
+        <f>M35-MAX(M$2:M35)</f>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1">
+        <f>N35-MAX(N$2:N35)</f>
+        <v>0</v>
+      </c>
+      <c r="R35" s="32">
+        <f>O35-MAX(O$2:O35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" thickBot="1">
       <c r="C36" s="23" t="s">
         <v>91</v>
       </c>
@@ -2371,46 +3261,78 @@
         <v>0.18142000000000003</v>
       </c>
       <c r="F36" s="11">
-        <f t="shared" ref="F36:H36" si="6">SUM(F2:F35)</f>
+        <f t="shared" ref="F36:H36" si="21">SUM(F2:F35)</f>
         <v>0.25799999999999995</v>
       </c>
       <c r="G36" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="21"/>
         <v>0.49179999999999996</v>
       </c>
       <c r="H36" s="10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="21"/>
         <v>2.7471399999999995</v>
       </c>
-      <c r="J36" s="38">
+      <c r="J36" s="36">
         <f>MAX(J2:J35)</f>
         <v>0.11149999999999999</v>
       </c>
-      <c r="K36" s="39">
-        <f t="shared" ref="K36:L36" si="7">MAX(K2:K35)</f>
+      <c r="K36" s="37">
+        <f t="shared" ref="K36:L36" si="22">MAX(K2:K35)</f>
         <v>0.1013</v>
       </c>
-      <c r="L36" s="40">
-        <f t="shared" si="7"/>
+      <c r="L36" s="38">
+        <f t="shared" si="22"/>
         <v>0.11890000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="15" thickBot="1"/>
-    <row r="38" spans="1:12" ht="15.75" thickBot="1">
-      <c r="C38" s="23" t="s">
+      <c r="P36" s="47">
+        <f>MIN(P2:P35)</f>
+        <v>-0.12117999999999998</v>
+      </c>
+      <c r="Q36" s="47">
+        <f t="shared" ref="Q36:R36" si="23">MIN(Q2:Q35)</f>
+        <v>-0.2263</v>
+      </c>
+      <c r="R36" s="47">
+        <f t="shared" si="23"/>
+        <v>-0.38300000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="15" thickBot="1"/>
+    <row r="38" spans="1:18" ht="15" thickBot="1">
+      <c r="C38" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="24">
+      <c r="D38" s="52" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="49">
         <f>E36/J36</f>
         <v>1.6270852017937223</v>
       </c>
-      <c r="F38" s="25">
-        <f t="shared" ref="F38:G38" si="8">F36/K36</f>
+      <c r="F38" s="50">
+        <f t="shared" ref="F38:G38" si="24">F36/K36</f>
         <v>2.5468904244817367</v>
       </c>
-      <c r="G38" s="26">
-        <f t="shared" si="8"/>
+      <c r="G38" s="51">
+        <f t="shared" si="24"/>
         <v>4.1362489486963829</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="15.75" thickBot="1">
+      <c r="C39" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E39" s="24">
+        <f>-E36/P36</f>
+        <v>1.4971117346096721</v>
+      </c>
+      <c r="F39" s="24">
+        <f t="shared" ref="F39:G39" si="25">-F36/Q36</f>
+        <v>1.1400795404330533</v>
+      </c>
+      <c r="G39" s="53">
+        <f t="shared" si="25"/>
+        <v>1.2840731070496083</v>
       </c>
     </row>
   </sheetData>
@@ -3935,7 +4857,7 @@
       <c r="B35" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="29" t="s">
         <v>39</v>
       </c>
       <c r="D35" s="5">

</xml_diff>

<commit_message>
[UPD] Wykresy zysku skumulowanego dla "konkursu"
</commit_message>
<xml_diff>
--- a/Results/AS/wyniki.xlsx
+++ b/Results/AS/wyniki.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21345" windowHeight="10110"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="21345" windowHeight="10110" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="wyniki" sheetId="1" r:id="rId1"/>
     <sheet name="Parametry" sheetId="2" r:id="rId2"/>
+    <sheet name="Wykresy" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="113">
   <si>
     <t>nr testu</t>
   </si>
@@ -342,6 +343,18 @@
   </si>
   <si>
     <t>źle liczony</t>
+  </si>
+  <si>
+    <t>DLA 100</t>
+  </si>
+  <si>
+    <t>DLA 200</t>
+  </si>
+  <si>
+    <t>DLA 500</t>
+  </si>
+  <si>
+    <t>WYNIK</t>
   </si>
 </sst>
 </file>
@@ -690,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -805,6 +818,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -812,6 +829,614 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>wyniki!$M$2:$M$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.61E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7899999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5399999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4399999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0099999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.6599999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.3400000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.121</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.7100000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.4000000000000029E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.5500000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.4300000000000014E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.4300000000000014E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.4620000000000015E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.352000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.2720000000000018E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.7999999999998226E-4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.4620000000000012E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0820000000000012E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.3720000000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.4520000000000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.4220000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.5520000000000009E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.2820000000000014E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.10402000000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.11152000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.10932000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.11932000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.13562000000000002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.15242000000000003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.18142000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="77989760"/>
+        <c:axId val="78004992"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="77989760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="78004992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="78004992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77989760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>wyniki!$N$2:$N$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>3.4700000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1699999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9599999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.12669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16539999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2026</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.214</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.19309999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18529999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.10189999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4799999999999989E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.8999999999999988E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.11159999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15039999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15059999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.15139999999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.10369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.7999999999999822E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.2300000000000018E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.6999999999999838E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.9999999999999836E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.7199999999999977E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.7699999999999972E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.6599999999999969E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.9399999999999974E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.12159999999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.14069999999999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.14599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.15729999999999997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.16639999999999996</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.18239999999999995</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.21909999999999996</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.25799999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="86537344"/>
+        <c:axId val="86538880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="86537344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="86538880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="86538880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="86537344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>wyniki!$O$2:$O$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>4.3999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.64E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1731</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23960000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.29510000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34110000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3609</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3054</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18630000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.16990000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.18760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.18420000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.29970000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.38800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.37090000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3019</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.24280000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.18400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.4000000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.0000000000000114E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.1800000000000012E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.10840000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.1704</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.17080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.20400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.25290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.29349999999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.33429999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.36709999999999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.37439999999999996</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.43239999999999995</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.49179999999999996</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.49179999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="86518016"/>
+        <c:axId val="86529152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="86518016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="86529152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="86529152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="86518016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Wykres 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1101,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E39" activeCellId="1" sqref="E36 E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4898,4 +5523,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:K27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="J24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="15">
+      <c r="K26" s="54">
+        <v>0.18142000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="15">
+      <c r="K27" s="55">
+        <v>1.4971117346096721</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>